<commit_message>
Setup Stage -> NDS
</commit_message>
<xml_diff>
--- a/Ontario_Covid/Report/NDS/Stage_NDS.xlsx
+++ b/Ontario_Covid/Report/NDS/Stage_NDS.xlsx
@@ -5,16 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\University\4th-year\HKI\BI\Thực hành\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\University\4th-year\HKI\BI\Thực hành\Project\Ontario_Covid\Ontario_Covid\Report\NDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA20DB8-ADEA-41B3-B080-C674659BE3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F138A47-AE79-4AF8-B527-C9030A3DAB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Trang_tính1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -127,7 +126,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -150,11 +149,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -162,6 +185,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -446,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -462,7 +492,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -473,7 +503,7 @@
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -484,7 +514,7 @@
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -495,7 +525,7 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -503,7 +533,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -517,7 +547,7 @@
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -528,7 +558,7 @@
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -539,7 +569,7 @@
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -550,16 +580,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52825273-67BB-4A2C-878D-4369254A5234}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>